<commit_message>
Collection of FlexTest 20mm
I collected 17 data points for the flexor muscle with a 20mm BPA
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_FullSize.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_FullSize.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason Miranda\Documents\GitHub\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323572DE-9FF6-4DE3-A3F9-402EDDF6A983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B7C418-247E-460F-AF9C-F418512DE028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtTest40mm" sheetId="2" r:id="rId1"/>
     <sheet name="FlxTest20mm" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,6 +26,7 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t>Test #</t>
   </si>
@@ -87,6 +88,27 @@
   </si>
   <si>
     <t>Flexor Test 20mm</t>
+  </si>
+  <si>
+    <t>tendon length</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>**</t>
+  </si>
+  <si>
+    <t>*Pipe Started to kink at 7</t>
+  </si>
+  <si>
+    <t>**Pressure stepped up from 300kPa to 500kPa on test 11-15</t>
+  </si>
+  <si>
+    <t>***Pressure stepped up from 500kPa to 620kPa on test 16</t>
+  </si>
+  <si>
+    <t>***</t>
   </si>
 </sst>
 </file>
@@ -599,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DDD6FA0-ED90-4B9F-A1DF-3E2DAEF07409}">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:K7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,7 +722,7 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>16.268999999999998</v>
+        <v>21.395</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -708,7 +730,7 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -719,7 +741,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="2">
-        <v>33.6</v>
+        <v>36.1</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -742,7 +764,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="16">
-        <v>30.5</v>
+        <v>32</v>
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="16"/>
@@ -765,7 +787,7 @@
         <v>3</v>
       </c>
       <c r="C10">
-        <v>518</v>
+        <v>533</v>
       </c>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
@@ -847,7 +869,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="16">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
@@ -870,7 +892,7 @@
       </c>
       <c r="C15">
         <f>C6*COS(RADIANS(C9-3.05))*C12/1000</f>
-        <v>5.284784415964447</v>
+        <v>6.8530172364026392</v>
       </c>
       <c r="D15">
         <f t="shared" ref="D15:K15" si="0">D6*COS(RADIANS(D9-3.05))*D12/1000</f>
@@ -937,16 +959,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F358BD-411F-4156-AA93-0DF96BD5C242}">
-  <dimension ref="A1:Q15"/>
+  <dimension ref="A1:X18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="W14" sqref="W14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="19.7109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" style="5" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" customWidth="1"/>
@@ -955,29 +977,50 @@
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C2">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C3">
         <f>C2-C2*0.17</f>
-        <v>344.45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <v>351.09</v>
+      </c>
+      <c r="M3">
+        <f>1-369.5/423</f>
+        <v>0.12647754137115841</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>17</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" t="s">
+        <v>20</v>
+      </c>
+      <c r="R4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>0</v>
       </c>
@@ -1026,24 +1069,126 @@
       <c r="Q5" s="12">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R5" s="12">
+        <v>16</v>
+      </c>
+      <c r="S5" s="12">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C6">
-        <v>23.454999999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+        <v>29.225000000000001</v>
+      </c>
+      <c r="D6">
+        <v>24.009</v>
+      </c>
+      <c r="E6">
+        <v>20.302</v>
+      </c>
+      <c r="F6">
+        <v>17.245999999999999</v>
+      </c>
+      <c r="G6">
+        <v>14.472</v>
+      </c>
+      <c r="H6">
+        <v>11.127000000000001</v>
+      </c>
+      <c r="I6">
+        <v>11.121</v>
+      </c>
+      <c r="J6">
+        <v>9.2840000000000007</v>
+      </c>
+      <c r="K6">
+        <v>6.8421000000000003</v>
+      </c>
+      <c r="L6">
+        <v>2.9257</v>
+      </c>
+      <c r="M6">
+        <v>19.082999999999998</v>
+      </c>
+      <c r="N6">
+        <v>14.757</v>
+      </c>
+      <c r="O6">
+        <v>11.612</v>
+      </c>
+      <c r="P6">
+        <v>5.8364000000000003</v>
+      </c>
+      <c r="Q6">
+        <v>3.1772</v>
+      </c>
+      <c r="R6">
+        <v>7.6226000000000003</v>
+      </c>
+      <c r="S6">
+        <v>4.8666</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>11.5</v>
+      </c>
+      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <v>27</v>
+      </c>
+      <c r="G7">
+        <v>35</v>
+      </c>
+      <c r="H7">
+        <v>44</v>
+      </c>
+      <c r="I7">
+        <v>54.5</v>
+      </c>
+      <c r="J7">
+        <v>50</v>
+      </c>
+      <c r="K7">
+        <v>63</v>
+      </c>
+      <c r="L7">
+        <v>64</v>
+      </c>
+      <c r="M7">
+        <v>73.5</v>
+      </c>
+      <c r="N7">
+        <v>82</v>
+      </c>
+      <c r="O7">
+        <v>88</v>
+      </c>
+      <c r="P7">
+        <v>103.5</v>
+      </c>
+      <c r="Q7">
+        <v>114</v>
+      </c>
+      <c r="R7">
+        <v>115</v>
+      </c>
+      <c r="S7">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
@@ -1051,70 +1196,182 @@
         <v>12</v>
       </c>
       <c r="C8" s="2">
-        <v>6</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="D8" s="4">
+        <v>21.4</v>
+      </c>
+      <c r="E8" s="4">
+        <v>22.3</v>
+      </c>
+      <c r="F8" s="4">
+        <v>23.1</v>
+      </c>
+      <c r="G8" s="4">
+        <v>24.9</v>
+      </c>
+      <c r="H8" s="4">
+        <v>28.4</v>
+      </c>
+      <c r="I8" s="4">
+        <v>29.3</v>
+      </c>
+      <c r="J8" s="4">
+        <v>29.4</v>
+      </c>
+      <c r="K8" s="4">
+        <v>35.1</v>
+      </c>
+      <c r="L8" s="4">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="M8" s="4">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="N8" s="4">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="O8" s="4">
+        <v>34.9</v>
+      </c>
+      <c r="P8" s="4">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>42.7</v>
+      </c>
+      <c r="R8" s="2">
+        <v>46.4</v>
+      </c>
+      <c r="S8" s="2">
+        <v>48.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
       <c r="B9" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="16">
-        <v>23</v>
-      </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
-    </row>
-    <row r="10" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>24.5</v>
+      </c>
+      <c r="D9" s="16">
+        <v>22</v>
+      </c>
+      <c r="E9" s="16">
+        <v>24</v>
+      </c>
+      <c r="F9" s="16">
+        <v>25.5</v>
+      </c>
+      <c r="G9" s="16">
+        <v>31.5</v>
+      </c>
+      <c r="H9" s="16">
+        <v>31</v>
+      </c>
+      <c r="I9" s="16">
+        <v>31.5</v>
+      </c>
+      <c r="J9" s="16">
+        <v>30</v>
+      </c>
+      <c r="K9" s="16">
+        <v>31.5</v>
+      </c>
+      <c r="L9" s="16">
+        <v>33.5</v>
+      </c>
+      <c r="M9" s="16">
+        <v>38.5</v>
+      </c>
+      <c r="N9" s="16">
+        <v>44.5</v>
+      </c>
+      <c r="O9" s="16">
+        <v>43</v>
+      </c>
+      <c r="P9" s="16">
+        <v>54.5</v>
+      </c>
+      <c r="Q9" s="16">
+        <v>55.5</v>
+      </c>
+      <c r="R9" s="16">
+        <v>52</v>
+      </c>
+      <c r="S9" s="16">
+        <v>55</v>
+      </c>
+      <c r="T9" s="17"/>
+      <c r="U9" s="17"/>
+      <c r="V9" s="17"/>
+      <c r="W9" s="17"/>
+      <c r="X9" s="17"/>
+    </row>
+    <row r="10" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
       <c r="B10" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C10">
-        <v>397</v>
-      </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+        <v>401</v>
+      </c>
+      <c r="D10" s="16">
+        <v>395</v>
+      </c>
+      <c r="E10" s="16">
+        <v>389</v>
+      </c>
+      <c r="F10" s="16">
+        <v>387</v>
+      </c>
+      <c r="G10" s="16">
+        <v>382</v>
+      </c>
+      <c r="H10" s="16">
+        <v>380</v>
+      </c>
+      <c r="I10" s="16">
+        <v>378</v>
+      </c>
+      <c r="J10" s="16">
+        <v>374.5</v>
+      </c>
+      <c r="K10" s="16">
+        <v>371.5</v>
+      </c>
+      <c r="L10" s="16">
+        <v>369.5</v>
+      </c>
+      <c r="M10" s="16">
+        <v>354</v>
+      </c>
+      <c r="N10" s="16">
+        <v>352.5</v>
+      </c>
+      <c r="O10" s="16">
+        <v>350.5</v>
+      </c>
+      <c r="P10" s="16">
+        <v>345</v>
+      </c>
+      <c r="Q10" s="16">
+        <v>343.5</v>
+      </c>
+      <c r="R10" s="3">
+        <v>338.5</v>
+      </c>
+      <c r="S10" s="3">
+        <v>339</v>
+      </c>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="17"/>
+      <c r="W10" s="17"/>
+      <c r="X10" s="17"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>8</v>
       </c>
@@ -1137,7 +1394,7 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
       <c r="B12" s="10" t="s">
         <v>10</v>
@@ -1187,94 +1444,162 @@
       <c r="Q12" s="16">
         <v>366.43</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R12" s="16">
+        <v>366.43</v>
+      </c>
+      <c r="S12" s="16">
+        <v>366.43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="16">
+        <v>45</v>
+      </c>
+      <c r="D13" s="16">
+        <v>47</v>
+      </c>
+      <c r="E13" s="16">
+        <v>51</v>
+      </c>
+      <c r="F13" s="16">
+        <v>45</v>
+      </c>
+      <c r="G13" s="16">
+        <v>40</v>
+      </c>
+      <c r="H13" s="16">
+        <v>37</v>
+      </c>
+      <c r="I13" s="16">
         <v>38</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-    </row>
-    <row r="14" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J13" s="16">
+        <v>39</v>
+      </c>
+      <c r="K13" s="16">
+        <v>36.5</v>
+      </c>
+      <c r="L13" s="16">
+        <v>35.5</v>
+      </c>
+      <c r="M13" s="16">
+        <v>30.5</v>
+      </c>
+      <c r="N13" s="16">
+        <v>20</v>
+      </c>
+      <c r="O13" s="16">
+        <v>22</v>
+      </c>
+      <c r="P13" s="16">
+        <v>16</v>
+      </c>
+      <c r="Q13" s="16">
+        <v>4.5</v>
+      </c>
+      <c r="R13" s="16">
+        <v>3</v>
+      </c>
+      <c r="S13" s="16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C15">
-        <f t="shared" ref="C15:Q15" si="0">C6*COS(RADIANS(C9-2.83))*C12/1000</f>
-        <v>8.0675396019501164</v>
+        <f t="shared" ref="C15:S15" si="0">C6*COS(RADIANS(C9-2.83))*C12/1000</f>
+        <v>9.9520752292838743</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.309776190397633</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.9372085405748338</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5.8312110803111104</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.6528169082585853</v>
       </c>
       <c r="H15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.5943174716264252</v>
       </c>
       <c r="I15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.5754544525113139</v>
       </c>
       <c r="J15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.0265514767141273</v>
       </c>
       <c r="K15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.199767728579054</v>
       </c>
       <c r="L15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.92210333898321939</v>
       </c>
       <c r="M15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5.6806977708149313</v>
       </c>
       <c r="N15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.0392598352753879</v>
       </c>
       <c r="O15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.2513783399694391</v>
       </c>
       <c r="P15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.3263579017259233</v>
       </c>
       <c r="Q15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.70598947320621186</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="0"/>
+        <v>1.826208161538696</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="0"/>
+        <v>1.0937153129886135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="O18" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Data Points for Flexor
I added Extensor test 2-12 to the datapool
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_FullSize.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_FullSize.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason Miranda\Documents\GitHub\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B7C418-247E-460F-AF9C-F418512DE028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7543B31-0466-448A-83A3-D97B41E2F874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
+    <workbookView xWindow="28830" yWindow="15" windowWidth="21600" windowHeight="11385" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtTest40mm" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
   <si>
     <t>Test #</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>***</t>
+  </si>
+  <si>
+    <t>*changed pressure from 100 kPa to 230 kPa</t>
   </si>
 </sst>
 </file>
@@ -619,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DDD6FA0-ED90-4B9F-A1DF-3E2DAEF07409}">
-  <dimension ref="A1:Q15"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,7 +650,7 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>520</v>
+        <v>557</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -656,7 +659,11 @@
       </c>
       <c r="C3">
         <f>C2-C2*0.17</f>
-        <v>431.6</v>
+        <v>462.31</v>
+      </c>
+      <c r="I3">
+        <f>1-I10/C2</f>
+        <v>5.5655296229802476E-2</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -666,6 +673,9 @@
       <c r="C4">
         <v>30</v>
       </c>
+      <c r="J4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
@@ -724,6 +734,39 @@
       <c r="C6">
         <v>21.395</v>
       </c>
+      <c r="D6">
+        <v>9.8042999999999996</v>
+      </c>
+      <c r="E6">
+        <v>5.4329000000000001</v>
+      </c>
+      <c r="F6">
+        <v>1.5627</v>
+      </c>
+      <c r="G6">
+        <v>3.1173000000000002</v>
+      </c>
+      <c r="H6">
+        <v>4.5189000000000004</v>
+      </c>
+      <c r="I6">
+        <v>1.1431</v>
+      </c>
+      <c r="J6">
+        <v>20.042999999999999</v>
+      </c>
+      <c r="K6">
+        <v>3.3938000000000001</v>
+      </c>
+      <c r="L6">
+        <v>4.0789999999999997</v>
+      </c>
+      <c r="M6">
+        <v>20.853000000000002</v>
+      </c>
+      <c r="N6">
+        <v>10.808999999999999</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
@@ -732,6 +775,39 @@
       <c r="C7">
         <v>117</v>
       </c>
+      <c r="D7">
+        <v>106</v>
+      </c>
+      <c r="E7">
+        <v>96</v>
+      </c>
+      <c r="F7">
+        <v>66.5</v>
+      </c>
+      <c r="G7">
+        <v>74.5</v>
+      </c>
+      <c r="H7">
+        <v>85.5</v>
+      </c>
+      <c r="I7">
+        <v>53.5</v>
+      </c>
+      <c r="J7">
+        <v>53.5</v>
+      </c>
+      <c r="K7">
+        <v>17</v>
+      </c>
+      <c r="L7">
+        <v>17</v>
+      </c>
+      <c r="M7">
+        <v>42.5</v>
+      </c>
+      <c r="N7">
+        <v>30</v>
+      </c>
     </row>
     <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -743,17 +819,39 @@
       <c r="C8" s="2">
         <v>36.1</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
+      <c r="D8" s="4">
+        <v>29</v>
+      </c>
+      <c r="E8" s="4">
+        <v>26.5</v>
+      </c>
+      <c r="F8" s="4">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="G8" s="4">
+        <v>31.2</v>
+      </c>
+      <c r="H8" s="4">
+        <v>27.6</v>
+      </c>
+      <c r="I8" s="4">
+        <v>33.6</v>
+      </c>
+      <c r="J8" s="4">
+        <v>36.5</v>
+      </c>
+      <c r="K8" s="4">
+        <v>36</v>
+      </c>
+      <c r="L8" s="4">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="M8" s="4">
+        <v>39.9</v>
+      </c>
+      <c r="N8" s="4">
+        <v>39.700000000000003</v>
+      </c>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
@@ -766,17 +864,39 @@
       <c r="C9" s="16">
         <v>32</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
+      <c r="D9" s="16">
+        <v>34.5</v>
+      </c>
+      <c r="E9" s="16">
+        <v>31</v>
+      </c>
+      <c r="F9" s="16">
+        <v>44.5</v>
+      </c>
+      <c r="G9" s="16">
+        <v>35.5</v>
+      </c>
+      <c r="H9" s="16">
+        <v>33</v>
+      </c>
+      <c r="I9" s="16">
+        <v>35.5</v>
+      </c>
+      <c r="J9" s="16">
+        <v>35</v>
+      </c>
+      <c r="K9" s="16">
+        <v>35</v>
+      </c>
+      <c r="L9" s="16">
+        <v>37</v>
+      </c>
+      <c r="M9" s="16">
+        <v>40.5</v>
+      </c>
+      <c r="N9" s="16">
+        <v>38</v>
+      </c>
       <c r="O9" s="16"/>
       <c r="P9" s="16"/>
       <c r="Q9" s="16"/>
@@ -789,17 +909,39 @@
       <c r="C10">
         <v>533</v>
       </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
+      <c r="D10" s="16">
+        <v>529.5</v>
+      </c>
+      <c r="E10" s="16">
+        <v>520</v>
+      </c>
+      <c r="F10" s="16">
+        <v>524</v>
+      </c>
+      <c r="G10" s="16">
+        <v>522</v>
+      </c>
+      <c r="H10" s="16">
+        <v>522</v>
+      </c>
+      <c r="I10" s="16">
+        <v>526</v>
+      </c>
+      <c r="J10" s="16">
+        <v>470</v>
+      </c>
+      <c r="K10" s="16">
+        <v>461</v>
+      </c>
+      <c r="L10" s="16">
+        <v>461</v>
+      </c>
+      <c r="M10" s="16">
+        <v>462</v>
+      </c>
+      <c r="N10" s="16">
+        <v>457</v>
+      </c>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
@@ -871,14 +1013,39 @@
       <c r="C13" s="16">
         <v>60</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
+      <c r="D13" s="16">
+        <v>65</v>
+      </c>
+      <c r="E13" s="16">
+        <v>57</v>
+      </c>
+      <c r="F13" s="16">
+        <v>73</v>
+      </c>
+      <c r="G13" s="16">
+        <v>62</v>
+      </c>
+      <c r="H13" s="16">
+        <v>67</v>
+      </c>
+      <c r="I13" s="16">
+        <v>74</v>
+      </c>
+      <c r="J13" s="16">
+        <v>65</v>
+      </c>
+      <c r="K13" s="16">
+        <v>70</v>
+      </c>
+      <c r="L13" s="16">
+        <v>75</v>
+      </c>
+      <c r="M13" s="16">
+        <v>62.5</v>
+      </c>
+      <c r="N13" s="16">
+        <v>69</v>
+      </c>
     </row>
     <row r="14" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
@@ -896,47 +1063,47 @@
       </c>
       <c r="D15">
         <f t="shared" ref="D15:K15" si="0">D6*COS(RADIANS(D9-3.05))*D12/1000</f>
-        <v>0</v>
+        <v>3.0616448382428998</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.7567434855432555</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.42875300427896085</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.96291824494655998</v>
       </c>
       <c r="H15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.4332513689040982</v>
       </c>
       <c r="I15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.35309782369307174</v>
       </c>
       <c r="J15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.2252989619399299</v>
       </c>
       <c r="K15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.0541046558415272</v>
       </c>
       <c r="L15">
         <f t="shared" ref="L15:Q15" si="1">L6*COS(RADIANS(L9-2.83))*L12/1000</f>
-        <v>0</v>
+        <v>1.235368116067078</v>
       </c>
       <c r="M15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6.0420429311128272</v>
       </c>
       <c r="N15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.2343374006094714</v>
       </c>
       <c r="O15">
         <f t="shared" si="1"/>
@@ -949,6 +1116,11 @@
       <c r="Q15">
         <f t="shared" si="1"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished 40mm Extensor test
ran ExtTest13. Results table FullSize is done. Extensor test has negative knee angle for flexion and positive for extension.
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_FullSize.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_FullSize.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason Miranda\Documents\GitHub\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7543B31-0466-448A-83A3-D97B41E2F874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EAC3116-91DF-475F-B6AF-640AC1860C1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28830" yWindow="15" windowWidth="21600" windowHeight="11385" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
+    <workbookView xWindow="-26745" yWindow="1230" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtTest40mm" sheetId="2" r:id="rId1"/>
     <sheet name="FlxTest20mm" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>Test #</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>*changed pressure from 100 kPa to 230 kPa</t>
+  </si>
+  <si>
+    <t>**Increased pressure to 380 kPa</t>
+  </si>
+  <si>
+    <t>Added pulley in system</t>
   </si>
 </sst>
 </file>
@@ -622,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DDD6FA0-ED90-4B9F-A1DF-3E2DAEF07409}">
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,6 +671,10 @@
         <f>1-I10/C2</f>
         <v>5.5655296229802476E-2</v>
       </c>
+      <c r="N3">
+        <f>1-N10/C2</f>
+        <v>0.17953321364452424</v>
+      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
@@ -676,6 +686,9 @@
       <c r="J4" t="s">
         <v>19</v>
       </c>
+      <c r="O4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
@@ -767,46 +780,58 @@
       <c r="N6">
         <v>10.808999999999999</v>
       </c>
+      <c r="O6">
+        <v>33.079000000000001</v>
+      </c>
+      <c r="P6">
+        <v>19.314</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C7">
-        <v>117</v>
+        <v>-117</v>
       </c>
       <c r="D7">
-        <v>106</v>
+        <v>-106</v>
       </c>
       <c r="E7">
-        <v>96</v>
+        <v>-96</v>
       </c>
       <c r="F7">
-        <v>66.5</v>
+        <v>-66.5</v>
       </c>
       <c r="G7">
-        <v>74.5</v>
+        <v>-74.5</v>
       </c>
       <c r="H7">
-        <v>85.5</v>
+        <v>-85.5</v>
       </c>
       <c r="I7">
-        <v>53.5</v>
+        <v>-53.5</v>
       </c>
       <c r="J7">
-        <v>53.5</v>
+        <v>-53.5</v>
       </c>
       <c r="K7">
-        <v>17</v>
+        <v>-17</v>
       </c>
       <c r="L7">
-        <v>17</v>
+        <v>-17</v>
       </c>
       <c r="M7">
-        <v>42.5</v>
+        <v>-42.5</v>
       </c>
       <c r="N7">
-        <v>30</v>
+        <v>-30</v>
+      </c>
+      <c r="O7">
+        <v>-6</v>
+      </c>
+      <c r="P7">
+        <v>6.5</v>
       </c>
     </row>
     <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -852,8 +877,12 @@
       <c r="N8" s="4">
         <v>39.700000000000003</v>
       </c>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
+      <c r="O8" s="4">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="P8" s="4">
+        <v>32.5</v>
+      </c>
       <c r="Q8" s="4"/>
     </row>
     <row r="9" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -897,8 +926,12 @@
       <c r="N9" s="16">
         <v>38</v>
       </c>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
+      <c r="O9" s="16">
+        <v>34</v>
+      </c>
+      <c r="P9" s="16">
+        <v>33.5</v>
+      </c>
       <c r="Q9" s="16"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -942,8 +975,12 @@
       <c r="N10" s="16">
         <v>457</v>
       </c>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
+      <c r="O10" s="16">
+        <v>440</v>
+      </c>
+      <c r="P10" s="16">
+        <v>430</v>
+      </c>
       <c r="Q10" s="1"/>
     </row>
     <row r="11" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1046,6 +1083,12 @@
       <c r="N13" s="16">
         <v>69</v>
       </c>
+      <c r="O13" s="16">
+        <v>60</v>
+      </c>
+      <c r="P13" s="16">
+        <v>64</v>
+      </c>
     </row>
     <row r="14" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
@@ -1107,11 +1150,11 @@
       </c>
       <c r="O15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10.360519153738428</v>
       </c>
       <c r="P15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6.0809498055103717</v>
       </c>
       <c r="Q15">
         <f t="shared" si="1"/>
@@ -1121,6 +1164,16 @@
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J16" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O18" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1133,8 +1186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F358BD-411F-4156-AA93-0DF96BD5C242}">
   <dimension ref="A1:X18"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="W14" sqref="W14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1764,13 +1817,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="13:18" x14ac:dyDescent="0.25">
       <c r="M17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="13:15" x14ac:dyDescent="0.25">
-      <c r="O18" t="s">
+    <row r="18" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="R18" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Prep for 40mm test
We setup the 40mm extensor test and see if it would explode or not. good news it didnt
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_FullSize.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_FullSize.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason Miranda\Documents\GitHub\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EAC3116-91DF-475F-B6AF-640AC1860C1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC3CF383-25B5-4EAB-B82A-53B7153296FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26745" yWindow="1230" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
+    <workbookView xWindow="3495" yWindow="2820" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
   <sheets>
-    <sheet name="ExtTest40mm" sheetId="2" r:id="rId1"/>
-    <sheet name="FlxTest20mm" sheetId="1" r:id="rId2"/>
+    <sheet name="ExtTest40mm_1" sheetId="2" r:id="rId1"/>
+    <sheet name="ExtTest40mm_2" sheetId="4" r:id="rId2"/>
+    <sheet name="FlxTest20mm" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="28">
   <si>
     <t>Test #</t>
   </si>
@@ -1183,10 +1184,368 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A3F4CC-F96C-44DD-922E-2824BD5D818E}">
+  <dimension ref="A1:Q18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="5"/>
+    <col min="2" max="2" width="25.140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="9" width="13.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <f>C2-C2*0.17</f>
+        <v>462.31</v>
+      </c>
+      <c r="I3">
+        <f>1-I10/C2</f>
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <f>1-N10/C2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
+      </c>
+      <c r="J4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="12">
+        <v>1</v>
+      </c>
+      <c r="D5" s="12">
+        <v>2</v>
+      </c>
+      <c r="E5" s="12">
+        <v>3</v>
+      </c>
+      <c r="F5" s="12">
+        <v>4</v>
+      </c>
+      <c r="G5" s="12">
+        <v>5</v>
+      </c>
+      <c r="H5" s="12">
+        <v>6</v>
+      </c>
+      <c r="I5" s="12">
+        <v>7</v>
+      </c>
+      <c r="J5" s="12">
+        <v>8</v>
+      </c>
+      <c r="K5" s="12">
+        <v>9</v>
+      </c>
+      <c r="L5" s="12">
+        <v>10</v>
+      </c>
+      <c r="M5" s="12">
+        <v>11</v>
+      </c>
+      <c r="N5" s="12">
+        <v>12</v>
+      </c>
+      <c r="O5" s="12">
+        <v>13</v>
+      </c>
+      <c r="P5" s="12">
+        <v>14</v>
+      </c>
+      <c r="Q5" s="12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B7" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+    </row>
+    <row r="9" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+      <c r="B9" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="1"/>
+    </row>
+    <row r="11" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="16">
+        <v>366.05</v>
+      </c>
+      <c r="D12" s="16">
+        <v>366.05</v>
+      </c>
+      <c r="E12" s="16">
+        <v>366.05</v>
+      </c>
+      <c r="F12" s="16">
+        <v>366.05</v>
+      </c>
+      <c r="G12" s="16">
+        <v>366.05</v>
+      </c>
+      <c r="H12" s="16">
+        <v>366.05</v>
+      </c>
+      <c r="I12" s="16">
+        <v>366.05</v>
+      </c>
+      <c r="J12" s="16">
+        <v>366.05</v>
+      </c>
+      <c r="K12" s="16">
+        <v>366.05</v>
+      </c>
+      <c r="L12" s="16">
+        <v>366.05</v>
+      </c>
+      <c r="M12" s="16">
+        <v>366.05</v>
+      </c>
+      <c r="N12" s="16">
+        <v>366.05</v>
+      </c>
+      <c r="O12" s="16">
+        <v>366.05</v>
+      </c>
+      <c r="P12" s="16">
+        <v>366.05</v>
+      </c>
+      <c r="Q12" s="16">
+        <v>366.05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+    </row>
+    <row r="14" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <f>C6*COS(RADIANS(C9-3.05))*C12/1000</f>
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ref="D15:K15" si="0">D6*COS(RADIANS(D9-3.05))*D12/1000</f>
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <f t="shared" ref="L15:Q15" si="1">L6*COS(RADIANS(L9-2.83))*L12/1000</f>
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F358BD-411F-4156-AA93-0DF96BD5C242}">
   <dimension ref="A1:X18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
created more figures for report
more and more and more figures
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_FullSize.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_FullSize.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81AB57E-5CEA-432C-A13F-DF678B7A1115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3EF2F83-027D-43AD-A49F-840B601E9C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
+    <workbookView xWindow="-26580" yWindow="1185" windowWidth="21600" windowHeight="11385" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtTest40mm_1" sheetId="2" r:id="rId1"/>
@@ -3030,8 +3030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DDD6FA0-ED90-4B9F-A1DF-3E2DAEF07409}">
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:P11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3568,11 +3568,11 @@
         <v>6</v>
       </c>
       <c r="C16">
-        <f t="shared" ref="C16:K16" si="1">C6*COS(RADIANS(C9-3.05))*C13/1000</f>
+        <f>C6*COS(RADIANS(C9-3.05))*C13/1000</f>
         <v>6.8530172364026392</v>
       </c>
       <c r="D16">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="C16:K16" si="1">D6*COS(RADIANS(D9-3.05))*D13/1000</f>
         <v>3.0616448382428998</v>
       </c>
       <c r="E16">
@@ -3628,27 +3628,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="10:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="J17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="10:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="O18" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="10:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="O19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="10:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B20" s="5">
+        <f>557+50.8</f>
+        <v>607.79999999999995</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="K21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="10:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="K22" t="s">
         <v>29</v>
       </c>
@@ -3659,7 +3665,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="10:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="K23">
         <v>2.163E-2</v>
       </c>
@@ -3670,12 +3676,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="10:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="K25" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="10:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="K26" t="s">
         <v>29</v>
       </c>
@@ -3686,7 +3692,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="10:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="K27">
         <v>3.7760000000000002E-2</v>
       </c>
@@ -3708,8 +3714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A3F4CC-F96C-44DD-922E-2824BD5D818E}">
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4052,15 +4058,15 @@
         <v>6</v>
       </c>
       <c r="C17">
-        <f>C6*COS(RADIANS(C10))*C14/1000</f>
-        <v>19.58607747422618</v>
+        <f>C6*COS(RADIANS(C10-4.2))*C14/1000</f>
+        <v>19.907124595290242</v>
       </c>
       <c r="D17">
-        <f t="shared" ref="D17:Q17" si="0">D6*COS(RADIANS(D10))*D14/1000</f>
-        <v>28.872222435198726</v>
+        <f>D6*COS(RADIANS(D10-5))*D14/1000</f>
+        <v>29.41782280346224</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D17:Q17" si="0">E6*COS(RADIANS(E10))*E14/1000</f>
         <v>0</v>
       </c>
       <c r="F17">
@@ -4192,7 +4198,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F358BD-411F-4156-AA93-0DF96BD5C242}">
   <dimension ref="A1:X19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="C11" sqref="C11:S11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added pictures of tests
For measurements of actual tendon length
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_FullSize.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_FullSize.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\GitHub\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2FF06711-5694-4719-963C-91F4B922F518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579D594E-B1F1-4A90-A768-E7B636A85DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
@@ -18,7 +18,6 @@
     <sheet name="FlxTest20mm" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3720,7 +3719,7 @@
   <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4154,8 +4153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F358BD-411F-4156-AA93-0DF96BD5C242}">
   <dimension ref="A1:X19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Working on flexor 20mm plot
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_FullSize.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_FullSize.xlsx
@@ -5,39 +5,29 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\GitHub\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10A6A9F4-8462-4DE6-AF11-DDC2D2A8C220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18288A1-EF49-415C-AB17-A3B3D6F8F07E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtTest40mm_1" sheetId="2" r:id="rId1"/>
     <sheet name="ExtTest40mm_2" sheetId="4" r:id="rId2"/>
     <sheet name="FlxTest20mm" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="43">
   <si>
     <t>Test #</t>
   </si>
@@ -341,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -359,6 +349,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2710,13 +2701,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>112395</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>136207</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>316230</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>29527</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3048,24 +3039,24 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1015625" style="3"/>
-    <col min="2" max="2" width="25.1015625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.3125" customWidth="1"/>
-    <col min="5" max="5" width="8.68359375" customWidth="1"/>
-    <col min="6" max="6" width="11.3125" customWidth="1"/>
-    <col min="7" max="7" width="13.3125" customWidth="1"/>
-    <col min="8" max="9" width="13.41796875" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="25.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="9" width="13.42578125" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -3073,7 +3064,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
@@ -3094,7 +3085,7 @@
         <v>0.17953321364452424</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>15</v>
       </c>
@@ -3108,7 +3099,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
@@ -3158,7 +3149,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
@@ -3205,7 +3196,7 @@
         <v>19.314</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>2</v>
       </c>
@@ -3252,7 +3243,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
@@ -3302,7 +3293,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="8" t="s">
         <v>13</v>
@@ -3350,7 +3341,7 @@
         <v>33.5</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="8" t="s">
         <v>3</v>
@@ -3398,7 +3389,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="8" t="s">
         <v>32</v>
@@ -3460,7 +3451,7 @@
         <v>0.22800718132854578</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>8</v>
       </c>
@@ -3468,7 +3459,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="8" t="s">
         <v>10</v>
@@ -3519,7 +3510,7 @@
         <v>366.05</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="8" t="s">
         <v>11</v>
@@ -3567,13 +3558,13 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>6</v>
       </c>
@@ -3638,22 +3629,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="J17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="O18" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="O19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>41</v>
       </c>
@@ -3661,7 +3652,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>6.1297215268519301</v>
       </c>
@@ -3669,7 +3660,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>2.7479725044346299</v>
       </c>
@@ -3683,7 +3674,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>1.5877091527759399</v>
       </c>
@@ -3697,12 +3688,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C24">
         <v>0.39396830053809201</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C25">
         <v>0.87997523971335201</v>
       </c>
@@ -3710,7 +3701,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>1.3017605698980601</v>
       </c>
@@ -3724,7 +3715,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>0.32710826122173697</v>
       </c>
@@ -3738,37 +3729,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C28">
         <v>5.7663175704745298</v>
       </c>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C29">
         <v>0.99793195771798704</v>
       </c>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C30">
         <v>1.17473937755851</v>
       </c>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C31">
         <v>5.6669972560913404</v>
       </c>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C32">
         <v>3.0532323371378101</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33">
         <v>9.8822570388584001</v>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34">
         <v>5.8339811315985299</v>
       </c>
@@ -3784,28 +3775,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A3F4CC-F96C-44DD-922E-2824BD5D818E}">
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1015625" style="3"/>
-    <col min="2" max="2" width="25.1015625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.3125" customWidth="1"/>
-    <col min="5" max="5" width="8.68359375" customWidth="1"/>
-    <col min="6" max="6" width="11.3125" customWidth="1"/>
-    <col min="7" max="7" width="13.3125" customWidth="1"/>
-    <col min="8" max="9" width="13.41796875" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="25.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="9" width="13.42578125" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -3813,7 +3804,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
@@ -3822,7 +3813,7 @@
         <v>462.31</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>15</v>
       </c>
@@ -3830,7 +3821,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
@@ -3880,7 +3871,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
@@ -3891,7 +3882,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>2</v>
       </c>
@@ -3902,7 +3893,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>33</v>
       </c>
@@ -3913,7 +3904,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>7</v>
       </c>
@@ -3924,7 +3915,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="8" t="s">
         <v>13</v>
@@ -3975,7 +3966,7 @@
         <v>14.6</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="8" t="s">
         <v>3</v>
@@ -3984,7 +3975,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="8" t="s">
         <v>34</v>
@@ -3994,7 +3985,7 @@
         <v>0.28366247755834828</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>8</v>
       </c>
@@ -4002,7 +3993,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="8" t="s">
         <v>10</v>
@@ -4053,7 +4044,7 @@
         <v>240.61</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="8" t="s">
         <v>11</v>
@@ -4062,13 +4053,13 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>6</v>
       </c>
@@ -4133,7 +4124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>27</v>
       </c>
@@ -4144,12 +4135,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>28</v>
       </c>
@@ -4160,7 +4151,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>29</v>
       </c>
@@ -4178,7 +4169,7 @@
         <v>18.260899999999999</v>
       </c>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>2.018E-2</v>
       </c>
@@ -4189,12 +4180,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>29</v>
       </c>
@@ -4208,7 +4199,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>3.619E-2</v>
       </c>
@@ -4227,30 +4218,30 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F358BD-411F-4156-AA93-0DF96BD5C242}">
-  <dimension ref="A1:X20"/>
+  <dimension ref="A1:X21"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1015625" style="3"/>
-    <col min="2" max="2" width="25.1015625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.3125" customWidth="1"/>
-    <col min="5" max="5" width="8.68359375" customWidth="1"/>
-    <col min="6" max="6" width="11.3125" customWidth="1"/>
-    <col min="7" max="7" width="13.3125" customWidth="1"/>
-    <col min="8" max="9" width="13.41796875" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="25.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="9" width="13.42578125" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -4258,7 +4249,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
@@ -4281,7 +4272,7 @@
         <v>0.12647754137115841</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>18</v>
       </c>
@@ -4298,7 +4289,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
@@ -4354,7 +4345,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
@@ -4410,7 +4401,7 @@
         <v>4.8666</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>2</v>
       </c>
@@ -4466,7 +4457,7 @@
         <v>-120</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
         <v>37</v>
       </c>
@@ -4522,7 +4513,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="9" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>7</v>
       </c>
@@ -4581,7 +4572,7 @@
         <v>48.1</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="8" t="s">
         <v>13</v>
@@ -4638,7 +4629,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="8" t="s">
         <v>3</v>
@@ -4700,7 +4691,7 @@
       <c r="W11"/>
       <c r="X11"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>8</v>
       </c>
@@ -4723,7 +4714,7 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="8" t="s">
         <v>10</v>
@@ -4780,7 +4771,7 @@
         <v>366.43</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="8" t="s">
         <v>11</v>
@@ -4837,13 +4828,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>6</v>
       </c>
@@ -4916,26 +4907,82 @@
         <v>-1.0937153129886135</v>
       </c>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="J17" t="s">
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B17" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17">
+        <v>-8.8432229117959409</v>
+      </c>
+      <c r="D17">
+        <v>-7.3877101457331502</v>
+      </c>
+      <c r="E17">
+        <v>-6.1229590706185704</v>
+      </c>
+      <c r="F17">
+        <v>-5.1141685562792896</v>
+      </c>
+      <c r="G17">
+        <v>-4.0057750611846901</v>
+      </c>
+      <c r="H17">
+        <v>-3.08271954812317</v>
+      </c>
+      <c r="I17">
+        <v>-3.0425145122501802</v>
+      </c>
+      <c r="J17">
+        <v>-2.5938436656752</v>
+      </c>
+      <c r="K17">
+        <v>-1.8617853154184101</v>
+      </c>
+      <c r="L17">
+        <v>-0.77484936807902705</v>
+      </c>
+      <c r="M17">
+        <v>-4.6544090914984197</v>
+      </c>
+      <c r="N17">
+        <v>-3.1970354025926402</v>
+      </c>
+      <c r="O17">
+        <v>-2.5796638217396901</v>
+      </c>
+      <c r="P17">
+        <v>-0.95909890934415098</v>
+      </c>
+      <c r="Q17">
+        <v>-0.49957241733930002</v>
+      </c>
+      <c r="R17">
+        <v>-1.3329952543772701</v>
+      </c>
+      <c r="S17">
+        <v>-0.77272430551831095</v>
+      </c>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="M18" t="s">
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="M19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="R19" t="s">
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B20" s="3" t="s">
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Getting ready for data collection
Need to adjust jig frame before collecting 20mm flexor data again.
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_FullSize.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_FullSize.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A13993E4-57D0-4583-9764-4E3899F6DC77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F2FC8A-F90B-42DB-A544-066DF8327768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtTest40mm_1" sheetId="2" r:id="rId1"/>
     <sheet name="ExtTest40mm_2" sheetId="4" r:id="rId2"/>
     <sheet name="FlxTest20mm_42cm" sheetId="1" r:id="rId3"/>
     <sheet name="FlxTest20mm_39cm" sheetId="5" r:id="rId4"/>
+    <sheet name="FlxTest20mm_39cm (2)" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="45">
   <si>
     <t>Test #</t>
   </si>
@@ -338,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -360,7 +361,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2163,6 +2163,616 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>20 mm Flexor Torque</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>500 kPA</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.11194116360454943"/>
+                  <c:y val="0.27785177894429863"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'FlxTest20mm_39cm (2)'!$M$7:$Q$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'FlxTest20mm_39cm (2)'!$M$16:$Q$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-73D8-4B82-9CE3-EACF8D22A23B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>300 kPa</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'FlxTest20mm_39cm (2)'!$C$7:$L$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-124</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-98.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-118.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-111</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-90</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'FlxTest20mm_39cm (2)'!$C$16:$L$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-5.6541833371388703</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-11.416082319316914</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-5.7080411596584568</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-10.218147814891781</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-13.937767935473495</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-17.298116513358377</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-20.398495906594288</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-73D8-4B82-9CE3-EACF8D22A23B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>620 kPa</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="5.8333333333333334E-2"/>
+                  <c:y val="0.37889690871974335"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'FlxTest20mm_39cm (2)'!$R$7:$S$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'FlxTest20mm_39cm (2)'!$R$16:$S$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-73D8-4B82-9CE3-EACF8D22A23B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1221401968"/>
+        <c:axId val="1221403632"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1221401968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1221403632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1221403632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1221401968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2283,6 +2893,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3316,6 +3966,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3934,6 +5100,49 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11E6C17D-4B38-4828-A3F0-A1D54F01A8F9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>112395</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>136207</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>316230</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>29527</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8470E9A2-F651-48E8-BE77-60E5337E068A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6217,7 +7426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AA058C6-A5F1-41EF-81BC-5D2D9F894F5C}">
   <dimension ref="A1:X21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
@@ -6450,25 +7659,25 @@
       <c r="B10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10">
         <v>29</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10">
         <v>31</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10">
         <v>31</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10">
         <v>27</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10">
         <v>28</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H10">
         <v>24</v>
       </c>
-      <c r="I10" s="19">
+      <c r="I10">
         <v>20</v>
       </c>
     </row>
@@ -6480,19 +7689,19 @@
       <c r="C11">
         <v>330</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11">
         <v>331</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11">
         <v>328</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11">
         <v>330</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11">
         <v>333</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H11">
         <v>337</v>
       </c>
       <c r="I11"/>
@@ -6543,49 +7752,49 @@
       <c r="C13">
         <v>350</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13">
         <v>350</v>
       </c>
-      <c r="E13" s="19">
+      <c r="E13">
         <v>350</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F13">
         <v>350</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G13">
         <v>350</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H13">
         <v>350</v>
       </c>
-      <c r="I13" s="19">
+      <c r="I13">
         <v>350</v>
       </c>
-      <c r="J13" s="19">
+      <c r="J13">
         <v>350</v>
       </c>
-      <c r="K13" s="19">
+      <c r="K13">
         <v>350</v>
       </c>
-      <c r="L13" s="19">
+      <c r="L13">
         <v>350</v>
       </c>
-      <c r="M13" s="19">
+      <c r="M13">
         <v>350</v>
       </c>
-      <c r="N13" s="19">
+      <c r="N13">
         <v>350</v>
       </c>
-      <c r="O13" s="19">
+      <c r="O13">
         <v>350</v>
       </c>
-      <c r="P13" s="19">
+      <c r="P13">
         <v>350</v>
       </c>
-      <c r="Q13" s="19">
+      <c r="Q13">
         <v>350</v>
       </c>
-      <c r="R13" s="19">
+      <c r="R13">
         <v>350</v>
       </c>
     </row>
@@ -6600,16 +7809,515 @@
       <c r="D14">
         <v>25</v>
       </c>
-      <c r="E14" s="19">
+      <c r="E14">
         <v>15</v>
       </c>
-      <c r="F14" s="19">
+      <c r="F14">
         <v>20</v>
       </c>
-      <c r="G14" s="19">
+      <c r="G14">
         <v>25</v>
       </c>
-      <c r="H14" s="19">
+      <c r="H14">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="B15" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <f>-C6*COS(RADIANS(C10-2.83))*C13/1000</f>
+        <v>-5.6541833371388703</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ref="D16:S16" si="0">-D6*COS(RADIANS(D10-2.83))*D13/1000</f>
+        <v>-11.416082319316914</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>-5.7080411596584568</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>-10.218147814891781</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>-13.937767935473495</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>-17.298116513358377</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>-20.398495906594288</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2201CA6F-EFE7-4253-8041-7C38B87FE418}">
+  <dimension ref="A1:X21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="25.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="9" width="13.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>390</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="16"/>
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <f>C2*(1-0.25)</f>
+        <v>292.5</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="17">
+        <v>289</v>
+      </c>
+      <c r="F3" s="18">
+        <f>(C2-E3)/C2</f>
+        <v>0.258974358974359</v>
+      </c>
+      <c r="G3">
+        <v>290</v>
+      </c>
+      <c r="H3">
+        <f>(C2-G3)/C2</f>
+        <v>0.25641025641025639</v>
+      </c>
+      <c r="M3">
+        <f>1-369.5/423</f>
+        <v>0.12647754137115841</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" t="s">
+        <v>20</v>
+      </c>
+      <c r="R4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="10">
+        <v>1</v>
+      </c>
+      <c r="D5" s="10">
+        <v>2</v>
+      </c>
+      <c r="E5" s="10">
+        <v>3</v>
+      </c>
+      <c r="F5" s="10">
+        <v>4</v>
+      </c>
+      <c r="G5" s="10">
+        <v>5</v>
+      </c>
+      <c r="H5" s="10">
+        <v>6</v>
+      </c>
+      <c r="I5" s="10">
+        <v>7</v>
+      </c>
+      <c r="J5" s="10">
+        <v>8</v>
+      </c>
+      <c r="K5" s="10">
+        <v>9</v>
+      </c>
+      <c r="L5" s="10">
+        <v>10</v>
+      </c>
+      <c r="M5" s="10">
+        <v>11</v>
+      </c>
+      <c r="N5" s="10">
+        <v>12</v>
+      </c>
+      <c r="O5" s="10">
+        <v>13</v>
+      </c>
+      <c r="P5" s="10">
+        <v>14</v>
+      </c>
+      <c r="Q5" s="10">
+        <v>15</v>
+      </c>
+      <c r="R5" s="10">
+        <v>16</v>
+      </c>
+      <c r="S5" s="10">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <v>37</v>
+      </c>
+      <c r="E6">
+        <v>18.5</v>
+      </c>
+      <c r="F6">
+        <v>32</v>
+      </c>
+      <c r="G6">
+        <v>44</v>
+      </c>
+      <c r="H6">
+        <v>53</v>
+      </c>
+      <c r="I6">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>-124</v>
+      </c>
+      <c r="D7">
+        <v>-98.5</v>
+      </c>
+      <c r="E7">
+        <v>-118.5</v>
+      </c>
+      <c r="F7">
+        <v>-111</v>
+      </c>
+      <c r="G7">
+        <v>-90</v>
+      </c>
+      <c r="H7">
+        <v>-75</v>
+      </c>
+      <c r="I7">
+        <v>-64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8">
+        <v>610</v>
+      </c>
+      <c r="D8">
+        <v>609</v>
+      </c>
+      <c r="E8">
+        <v>608.75</v>
+      </c>
+      <c r="F8">
+        <v>608</v>
+      </c>
+      <c r="G8">
+        <v>608</v>
+      </c>
+      <c r="H8">
+        <v>608</v>
+      </c>
+      <c r="I8">
+        <v>606.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>29</v>
+      </c>
+      <c r="D10">
+        <v>31</v>
+      </c>
+      <c r="E10">
+        <v>31</v>
+      </c>
+      <c r="F10">
+        <v>27</v>
+      </c>
+      <c r="G10">
+        <v>28</v>
+      </c>
+      <c r="H10">
+        <v>24</v>
+      </c>
+      <c r="I10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>330</v>
+      </c>
+      <c r="D11">
+        <v>331</v>
+      </c>
+      <c r="E11">
+        <v>328</v>
+      </c>
+      <c r="F11">
+        <v>330</v>
+      </c>
+      <c r="G11">
+        <v>333</v>
+      </c>
+      <c r="H11">
+        <v>337</v>
+      </c>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
+      <c r="P11"/>
+      <c r="Q11"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11"/>
+      <c r="W11"/>
+      <c r="X11"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+      <c r="B13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>350</v>
+      </c>
+      <c r="D13">
+        <v>350</v>
+      </c>
+      <c r="E13">
+        <v>350</v>
+      </c>
+      <c r="F13">
+        <v>350</v>
+      </c>
+      <c r="G13">
+        <v>350</v>
+      </c>
+      <c r="H13">
+        <v>350</v>
+      </c>
+      <c r="I13">
+        <v>350</v>
+      </c>
+      <c r="J13">
+        <v>350</v>
+      </c>
+      <c r="K13">
+        <v>350</v>
+      </c>
+      <c r="L13">
+        <v>350</v>
+      </c>
+      <c r="M13">
+        <v>350</v>
+      </c>
+      <c r="N13">
+        <v>350</v>
+      </c>
+      <c r="O13">
+        <v>350</v>
+      </c>
+      <c r="P13">
+        <v>350</v>
+      </c>
+      <c r="Q13">
+        <v>350</v>
+      </c>
+      <c r="R13">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>25</v>
+      </c>
+      <c r="E14">
+        <v>15</v>
+      </c>
+      <c r="F14">
+        <v>20</v>
+      </c>
+      <c r="G14">
+        <v>25</v>
+      </c>
+      <c r="H14">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Broke femur, needs redesign
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_FullSize.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_FullSize.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4887AC14-0C9D-4BDF-9716-1FB5D8304AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6448B3C3-BD82-471F-8AB9-B4C5FA93AC87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtTest40mm_1" sheetId="2" r:id="rId1"/>
@@ -18,8 +18,10 @@
     <sheet name="FlxTest20mm_42cm" sheetId="1" r:id="rId3"/>
     <sheet name="FlxTest20mm_39cm" sheetId="5" r:id="rId4"/>
     <sheet name="FlxTest20mm_39cm (2)" sheetId="6" r:id="rId5"/>
+    <sheet name="FlxTest20mm_42cm (2)" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="46">
   <si>
     <t>Test #</t>
   </si>
@@ -2767,6 +2769,619 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>20 mm Flexor Torque</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>500 kPA</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.11194116360454943"/>
+                  <c:y val="0.27785177894429863"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'FlxTest20mm_42cm (2)'!$M$7:$Q$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'FlxTest20mm_42cm (2)'!$M$16:$Q$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9313-468C-8F06-35E5A7DB46F3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>300 kPa</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'FlxTest20mm_42cm (2)'!$C$7:$L$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-125</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-112</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-93</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-75</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-52</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-42</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'FlxTest20mm_42cm (2)'!$C$16:$L$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-1.5702056777668703</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-6.0305367147524738</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-10.049415693445349</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-14.462104379205506</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-18.54620852024544</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-22.519923786080557</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-25.525501816571964</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-26.999475495745692</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-9313-468C-8F06-35E5A7DB46F3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>620 kPa</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="5.8333333333333334E-2"/>
+                  <c:y val="0.37889690871974335"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'FlxTest20mm_42cm (2)'!$R$7:$S$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'FlxTest20mm_42cm (2)'!$R$16:$S$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-9313-468C-8F06-35E5A7DB46F3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1221401968"/>
+        <c:axId val="1221403632"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1221401968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1221403632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1221403632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1221401968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2927,6 +3542,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4476,6 +5131,522 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5137,6 +6308,49 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8470E9A2-F651-48E8-BE77-60E5337E068A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>112395</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>136207</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>316230</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>29527</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22B2BFE5-CF05-416F-8D71-81AC0654865D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7919,8 +9133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2201CA6F-EFE7-4253-8041-7C38B87FE418}">
   <dimension ref="A1:X21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8363,4 +9577,525 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3C0B61-7108-442E-B33C-1C6DD21F395D}">
+  <dimension ref="A1:X21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="25.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="9" width="13.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>420</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="16"/>
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <f>C2*(1-0.25)</f>
+        <v>315</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="17"/>
+      <c r="F3" s="18">
+        <f>(C2-E3)/C2</f>
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <f>(C2-G3)/C2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="10">
+        <v>1</v>
+      </c>
+      <c r="D5" s="10">
+        <v>2</v>
+      </c>
+      <c r="E5" s="10">
+        <v>3</v>
+      </c>
+      <c r="F5" s="10">
+        <v>4</v>
+      </c>
+      <c r="G5" s="10">
+        <v>5</v>
+      </c>
+      <c r="H5" s="10">
+        <v>6</v>
+      </c>
+      <c r="I5" s="10">
+        <v>7</v>
+      </c>
+      <c r="J5" s="10">
+        <v>8</v>
+      </c>
+      <c r="K5" s="10">
+        <v>9</v>
+      </c>
+      <c r="L5" s="10">
+        <v>10</v>
+      </c>
+      <c r="M5" s="10">
+        <v>11</v>
+      </c>
+      <c r="N5" s="10">
+        <v>12</v>
+      </c>
+      <c r="O5" s="10">
+        <v>13</v>
+      </c>
+      <c r="P5" s="10">
+        <v>14</v>
+      </c>
+      <c r="Q5" s="10">
+        <v>15</v>
+      </c>
+      <c r="R5" s="10">
+        <v>16</v>
+      </c>
+      <c r="S5" s="10">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>5.3</v>
+      </c>
+      <c r="D6">
+        <v>19.829999999999998</v>
+      </c>
+      <c r="E6">
+        <v>31.35</v>
+      </c>
+      <c r="F6">
+        <v>44.78</v>
+      </c>
+      <c r="G6">
+        <v>56.1</v>
+      </c>
+      <c r="H6">
+        <v>68.12</v>
+      </c>
+      <c r="I6">
+        <v>74.900000000000006</v>
+      </c>
+      <c r="J6">
+        <v>78.14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>-125</v>
+      </c>
+      <c r="D7">
+        <v>-112</v>
+      </c>
+      <c r="E7">
+        <v>-93</v>
+      </c>
+      <c r="F7">
+        <v>-80</v>
+      </c>
+      <c r="G7">
+        <v>-75</v>
+      </c>
+      <c r="H7">
+        <v>-52</v>
+      </c>
+      <c r="I7">
+        <v>-42</v>
+      </c>
+      <c r="J7">
+        <v>-32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8">
+        <v>614</v>
+      </c>
+      <c r="D8">
+        <v>613.57000000000005</v>
+      </c>
+      <c r="E8">
+        <v>613.57000000000005</v>
+      </c>
+      <c r="F8">
+        <v>618</v>
+      </c>
+      <c r="G8">
+        <v>617</v>
+      </c>
+      <c r="H8">
+        <v>615</v>
+      </c>
+      <c r="I8">
+        <v>618</v>
+      </c>
+      <c r="J8">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>35</v>
+      </c>
+      <c r="D10">
+        <v>32.5</v>
+      </c>
+      <c r="E10">
+        <v>26.5</v>
+      </c>
+      <c r="F10">
+        <v>25.5</v>
+      </c>
+      <c r="G10">
+        <v>22</v>
+      </c>
+      <c r="H10">
+        <v>22</v>
+      </c>
+      <c r="I10">
+        <v>16</v>
+      </c>
+      <c r="J10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>330</v>
+      </c>
+      <c r="D11">
+        <v>335</v>
+      </c>
+      <c r="E11">
+        <v>339</v>
+      </c>
+      <c r="F11">
+        <v>345</v>
+      </c>
+      <c r="G11">
+        <v>350</v>
+      </c>
+      <c r="H11">
+        <v>355</v>
+      </c>
+      <c r="I11">
+        <v>357</v>
+      </c>
+      <c r="J11">
+        <v>360</v>
+      </c>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
+      <c r="P11"/>
+      <c r="Q11"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11"/>
+      <c r="W11"/>
+      <c r="X11"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+      <c r="B13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>350</v>
+      </c>
+      <c r="D13">
+        <v>350</v>
+      </c>
+      <c r="E13">
+        <v>350</v>
+      </c>
+      <c r="F13">
+        <v>350</v>
+      </c>
+      <c r="G13">
+        <v>350</v>
+      </c>
+      <c r="H13">
+        <v>350</v>
+      </c>
+      <c r="I13">
+        <v>350</v>
+      </c>
+      <c r="J13">
+        <v>350</v>
+      </c>
+      <c r="K13">
+        <v>350</v>
+      </c>
+      <c r="L13">
+        <v>350</v>
+      </c>
+      <c r="M13">
+        <v>350</v>
+      </c>
+      <c r="N13">
+        <v>350</v>
+      </c>
+      <c r="O13">
+        <v>350</v>
+      </c>
+      <c r="P13">
+        <v>350</v>
+      </c>
+      <c r="Q13">
+        <v>350</v>
+      </c>
+      <c r="R13">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <v>20</v>
+      </c>
+      <c r="D14">
+        <v>25</v>
+      </c>
+      <c r="E14">
+        <v>30</v>
+      </c>
+      <c r="F14">
+        <v>37</v>
+      </c>
+      <c r="G14">
+        <v>40</v>
+      </c>
+      <c r="H14">
+        <v>45</v>
+      </c>
+      <c r="I14">
+        <v>45</v>
+      </c>
+      <c r="J14">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="B15" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <f>-C6*COS(RADIANS(C10-2.83))*C13/1000</f>
+        <v>-1.5702056777668703</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ref="D16:S16" si="0">-D6*COS(RADIANS(D10-2.83))*D13/1000</f>
+        <v>-6.0305367147524738</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>-10.049415693445349</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>-14.462104379205506</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>-18.54620852024544</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>-22.519923786080557</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>-25.525501816571964</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>-26.999475495745692</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17">
+        <v>-1.5952</v>
+      </c>
+      <c r="D17">
+        <v>-6.0761000000000003</v>
+      </c>
+      <c r="E17">
+        <v>-10.005800000000001</v>
+      </c>
+      <c r="F17">
+        <v>-14.3527</v>
+      </c>
+      <c r="G17">
+        <v>-18.338999999999999</v>
+      </c>
+      <c r="H17">
+        <v>-22.190799999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Gettting this to work
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_FullSize.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_FullSize.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8722963-B816-4D4A-A7B4-09A7E638C19D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D65E96-6560-4404-80AD-2E765E5D9D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="6" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
@@ -213,15 +213,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAFCAFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCEBBDD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -361,11 +373,109 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -387,12 +497,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCEBBDD"/>
+      <color rgb="FFAFCAFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -3510,10 +3644,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>-26</c:v>
+                  <c:v>-26.01</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-26</c:v>
+                  <c:v>-26.001000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>-18.5</c:v>
@@ -3680,10 +3814,10 @@
                   <c:v>-55.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-53</c:v>
+                  <c:v>-53.000999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-53</c:v>
+                  <c:v>-53.01</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>-41</c:v>
@@ -9085,7 +9219,7 @@
   <dimension ref="A1:X21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10811,7 +10945,7 @@
   <dimension ref="A1:X21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11331,8 +11465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B5784E-5F9E-4AE8-9F2F-3ECBE91B1B37}">
   <dimension ref="A1:AD21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T28" sqref="T28"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11393,12 +11527,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C4">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
         <v>38</v>
@@ -11413,552 +11547,583 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:30" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+    <row r="5" spans="1:30" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="24"/>
+      <c r="B5" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="26">
         <v>1</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="26">
         <v>2</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="26">
         <v>3</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="26">
         <v>4</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="26">
         <v>5</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="26">
         <v>6</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="26">
         <v>7</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="26">
         <v>8</v>
       </c>
-      <c r="K5" s="10">
+      <c r="K5" s="27">
         <v>9</v>
       </c>
-      <c r="L5" s="10">
+      <c r="L5" s="27">
         <v>10</v>
       </c>
-      <c r="M5" s="10">
+      <c r="M5" s="27">
         <v>11</v>
       </c>
-      <c r="N5" s="10">
+      <c r="N5" s="27">
         <v>12</v>
       </c>
-      <c r="O5" s="10">
+      <c r="O5" s="27">
         <v>13</v>
       </c>
-      <c r="P5" s="10">
+      <c r="P5" s="27">
         <v>14</v>
       </c>
-      <c r="Q5" s="10">
+      <c r="Q5" s="27">
         <v>15</v>
       </c>
-      <c r="R5" s="10">
+      <c r="R5" s="27">
         <v>16</v>
       </c>
-      <c r="S5" s="10">
+      <c r="S5" s="27">
         <v>17</v>
       </c>
-      <c r="T5" s="10">
+      <c r="T5" s="27">
         <v>18</v>
       </c>
-      <c r="U5" s="10">
+      <c r="U5" s="26">
         <v>19</v>
       </c>
-      <c r="V5" s="10">
+      <c r="V5" s="26">
         <v>20</v>
       </c>
-      <c r="W5" s="10">
+      <c r="W5" s="26">
         <v>21</v>
       </c>
-      <c r="X5" s="10">
+      <c r="X5" s="26">
         <v>22</v>
       </c>
-      <c r="Y5" s="10">
+      <c r="Y5" s="28">
         <v>23</v>
       </c>
-      <c r="Z5" s="10">
+      <c r="Z5" s="28">
         <v>23</v>
       </c>
-      <c r="AA5" s="10">
+      <c r="AA5" s="28">
         <v>23</v>
       </c>
-      <c r="AB5" s="10">
+      <c r="AB5" s="28">
         <v>23</v>
       </c>
-      <c r="AC5" s="10">
+      <c r="AC5" s="28">
         <v>23</v>
       </c>
-      <c r="AD5" s="10">
+      <c r="AD5" s="28">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="22">
         <v>18.5</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="22">
         <v>18.05</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="22">
         <v>32</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="22">
         <v>40.97</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="22">
         <v>44.4</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="22">
         <v>50.84</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="22">
         <v>62.45</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="22">
         <v>69.400000000000006</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="23">
         <v>91.7</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="23">
         <v>114.1</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="23">
         <v>129.80000000000001</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="23">
         <v>78</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="23">
         <v>92.78</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="23">
         <v>63.6</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="23">
         <v>97.28</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="23">
         <v>71.92</v>
       </c>
-      <c r="S6">
+      <c r="S6" s="23">
         <v>84.5</v>
       </c>
-      <c r="T6">
+      <c r="T6" s="23">
         <v>93.9</v>
       </c>
-      <c r="U6">
+      <c r="U6" s="22">
         <v>64.3</v>
       </c>
-      <c r="V6">
+      <c r="V6" s="22">
         <v>70.599999999999994</v>
       </c>
-      <c r="W6">
+      <c r="W6" s="22">
         <v>90.15</v>
       </c>
-      <c r="X6">
+      <c r="X6" s="22">
         <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="20">
         <v>-125</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="20">
         <v>-114</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="20">
         <v>-98</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="20">
         <v>-83</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="20">
         <v>-75.5</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="20">
         <v>-69</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="20">
         <v>-55.5</v>
       </c>
-      <c r="J7">
-        <v>-53</v>
-      </c>
-      <c r="K7">
-        <v>-53</v>
-      </c>
-      <c r="L7">
+      <c r="J7" s="20">
+        <v>-53.000999999999998</v>
+      </c>
+      <c r="K7" s="21">
+        <v>-53.01</v>
+      </c>
+      <c r="L7" s="21">
         <v>-41</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="21">
         <v>-30</v>
       </c>
-      <c r="N7">
-        <v>-26</v>
-      </c>
-      <c r="O7">
-        <v>-26</v>
-      </c>
-      <c r="P7">
+      <c r="N7" s="21">
+        <v>-26.01</v>
+      </c>
+      <c r="O7" s="21">
+        <v>-26.001000000000001</v>
+      </c>
+      <c r="P7" s="21">
         <v>-18.5</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="21">
         <v>-18</v>
       </c>
-      <c r="R7">
+      <c r="R7" s="21">
         <v>-7</v>
       </c>
-      <c r="S7">
+      <c r="S7" s="21">
         <v>-9</v>
       </c>
-      <c r="T7">
+      <c r="T7" s="21">
         <v>0</v>
       </c>
-      <c r="U7">
+      <c r="U7" s="20">
         <v>3</v>
       </c>
-      <c r="V7">
+      <c r="V7" s="20">
         <v>7.7</v>
       </c>
-      <c r="W7">
+      <c r="W7" s="20">
         <v>-6.5</v>
       </c>
-      <c r="X7">
+      <c r="X7" s="20">
         <v>-32</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+    <row r="8" spans="1:30" s="34" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="30"/>
+      <c r="B8" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="32">
         <v>613</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="32">
         <v>614</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="32">
         <v>614</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="32">
         <v>615</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="32">
         <v>615</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="32">
         <v>615</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="32">
         <v>618</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="32">
         <v>618</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="33">
         <v>620</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="33">
         <v>620</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="33">
         <v>620</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="33">
         <v>385</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="33">
         <v>451</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="33">
         <v>296.60000000000002</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="33">
         <v>421</v>
       </c>
-      <c r="R8">
+      <c r="R8" s="33">
         <v>281</v>
       </c>
-      <c r="S8">
+      <c r="S8" s="33">
         <v>324.8</v>
       </c>
-      <c r="T8">
+      <c r="T8" s="33">
         <v>325.58</v>
       </c>
-      <c r="U8">
+      <c r="U8" s="32">
         <v>325.58</v>
       </c>
-      <c r="V8">
+      <c r="V8" s="32">
         <v>325</v>
       </c>
-      <c r="W8">
+      <c r="W8" s="32">
         <v>500</v>
       </c>
-      <c r="X8">
+      <c r="X8" s="32">
         <v>560</v>
       </c>
     </row>
-    <row r="9" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+    <row r="9" spans="1:30" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="19" t="s">
         <v>12</v>
       </c>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23"/>
+      <c r="T9" s="23"/>
+      <c r="U9" s="22"/>
+      <c r="V9" s="22"/>
+      <c r="W9" s="22"/>
+      <c r="X9" s="22"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="20">
         <v>32.5</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="20">
         <v>30</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="20">
         <v>28</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="20">
         <v>26</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="20">
         <v>24.5</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="20">
         <v>17</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="20">
         <v>20</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="20">
         <v>24</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="21">
         <v>-5</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="21">
         <v>-7</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="21">
         <v>-12</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="21">
         <v>-12</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="21">
         <v>-12</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="21">
         <v>-16.5</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="21">
         <v>-15</v>
       </c>
-      <c r="R10">
+      <c r="R10" s="21">
         <v>-19.5</v>
       </c>
-      <c r="S10">
+      <c r="S10" s="21">
         <v>-15</v>
       </c>
-      <c r="T10">
+      <c r="T10" s="21">
         <v>-17</v>
       </c>
-      <c r="U10">
+      <c r="U10" s="20">
         <v>7</v>
       </c>
-      <c r="V10">
+      <c r="V10" s="20">
         <v>5.5</v>
       </c>
-      <c r="W10">
+      <c r="W10" s="20">
         <v>10</v>
       </c>
-      <c r="X10">
+      <c r="X10" s="20">
         <v>13.5</v>
       </c>
     </row>
-    <row r="11" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="8" t="s">
+    <row r="11" spans="1:30" s="36" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="35"/>
+      <c r="B11" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="32">
         <v>334</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="32">
         <v>334</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="32">
         <v>338</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="32">
         <v>343</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="32">
         <v>348</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="32">
         <v>356</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="32">
         <v>356</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="33">
         <v>357</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="33">
         <v>365</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="33">
         <v>368</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="33">
         <v>381</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="33">
         <v>377</v>
       </c>
-      <c r="P11">
+      <c r="P11" s="33">
         <v>387</v>
       </c>
-      <c r="Q11">
+      <c r="Q11" s="33">
         <v>385</v>
       </c>
-      <c r="R11" s="2">
+      <c r="R11" s="33">
         <v>396</v>
       </c>
-      <c r="S11" s="2">
+      <c r="S11" s="33">
         <v>392</v>
       </c>
-      <c r="T11" s="2">
+      <c r="T11" s="33">
         <v>397</v>
       </c>
-      <c r="U11" s="2">
+      <c r="U11" s="32">
         <v>398</v>
       </c>
-      <c r="V11">
+      <c r="V11" s="32">
         <v>401</v>
       </c>
-      <c r="W11">
+      <c r="W11" s="32">
         <v>384</v>
       </c>
-      <c r="X11">
+      <c r="X11" s="32">
         <v>367</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="23"/>
+      <c r="R12" s="23"/>
+      <c r="S12" s="23"/>
+      <c r="T12" s="23"/>
+      <c r="U12" s="22"/>
+      <c r="V12" s="22"/>
+      <c r="W12" s="22"/>
+      <c r="X12" s="22"/>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="20">
         <v>350</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="20">
         <v>350</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="20">
         <v>350</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="20">
         <v>350</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="20">
         <v>350</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="20">
         <v>350</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="20">
         <v>350</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="20">
         <v>350</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="21">
         <v>255</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="21">
         <v>255</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="21">
         <v>255</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="21">
         <v>255</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="21">
         <v>255</v>
       </c>
-      <c r="P13">
+      <c r="P13" s="21">
         <v>255</v>
       </c>
-      <c r="Q13">
+      <c r="Q13" s="21">
         <v>255</v>
       </c>
-      <c r="R13">
+      <c r="R13" s="21">
         <v>255</v>
       </c>
-      <c r="S13">
+      <c r="S13" s="21">
         <v>255</v>
       </c>
-      <c r="T13">
+      <c r="T13" s="21">
         <v>255</v>
       </c>
-      <c r="U13">
+      <c r="U13" s="20">
         <v>350</v>
       </c>
-      <c r="V13">
+      <c r="V13" s="20">
         <v>350</v>
       </c>
-      <c r="W13">
+      <c r="W13" s="20">
         <v>350</v>
       </c>
-      <c r="X13">
+      <c r="X13" s="20">
         <v>350</v>
       </c>
       <c r="Y13">
@@ -11982,171 +12147,193 @@
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="20">
         <v>25</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="20">
         <v>25</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="20">
         <v>35</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="20">
         <v>35</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="20">
         <v>37</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="20">
         <v>40</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="20">
         <v>45</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="21">
         <v>48</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="21">
         <v>45</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="21">
         <v>40</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="21">
         <v>40</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="21">
         <v>40</v>
       </c>
-      <c r="P14">
+      <c r="P14" s="21">
         <v>42</v>
       </c>
-      <c r="Q14">
+      <c r="Q14" s="21">
         <v>45</v>
       </c>
-      <c r="R14">
+      <c r="R14" s="21">
         <v>46</v>
       </c>
-      <c r="S14">
+      <c r="S14" s="21">
         <v>48</v>
       </c>
-      <c r="T14">
+      <c r="T14" s="21">
         <v>48</v>
       </c>
-      <c r="U14">
+      <c r="U14" s="20">
         <v>42</v>
       </c>
-      <c r="V14">
+      <c r="V14" s="20">
         <v>43</v>
       </c>
-      <c r="W14">
+      <c r="W14" s="20">
         <v>45</v>
       </c>
-      <c r="X14">
+      <c r="X14" s="20">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="9" t="s">
+    <row r="15" spans="1:30" s="34" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="35"/>
+      <c r="B15" s="30" t="s">
         <v>4</v>
       </c>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="33"/>
+      <c r="M15" s="33"/>
+      <c r="N15" s="33"/>
+      <c r="O15" s="33"/>
+      <c r="P15" s="33"/>
+      <c r="Q15" s="33"/>
+      <c r="R15" s="33"/>
+      <c r="S15" s="33"/>
+      <c r="T15" s="33"/>
+      <c r="U15" s="32"/>
+      <c r="V15" s="32"/>
+      <c r="W15" s="32"/>
+      <c r="X15" s="32"/>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="22">
         <f>-C6*COS(RADIANS(C10-2.83))*C13/1000</f>
         <v>-5.6260680394816323</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="22">
         <f t="shared" ref="D16:AD16" si="0">-D6*COS(RADIANS(D10-2.83))*D13/1000</f>
         <v>-5.620399172616299</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="22">
         <f t="shared" si="0"/>
         <v>-10.136558498526179</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="22">
         <f t="shared" si="0"/>
         <v>-13.182897163275499</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="22">
         <f t="shared" si="0"/>
         <v>-14.441726709946776</v>
       </c>
-      <c r="H16">
-        <f t="shared" si="0"/>
+      <c r="H16" s="22">
+        <f>-H6*COS(RADIANS(H10-2.83))*H13/1000</f>
         <v>-17.25259369975322</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="22">
         <f t="shared" si="0"/>
         <v>-20.883378186341204</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="22">
         <f t="shared" si="0"/>
         <v>-22.6507412457938</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="23">
         <f t="shared" si="0"/>
         <v>-23.16548730865841</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="23">
         <f t="shared" si="0"/>
         <v>-28.66833854611783</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="23">
         <f t="shared" si="0"/>
         <v>-31.996455925810519</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="23">
         <f t="shared" si="0"/>
         <v>-19.227454254339136</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="23">
         <f t="shared" si="0"/>
         <v>-22.870810329712633</v>
       </c>
-      <c r="P16">
+      <c r="P16" s="23">
         <f t="shared" si="0"/>
         <v>-15.303755097401908</v>
       </c>
-      <c r="Q16">
+      <c r="Q16" s="23">
         <f t="shared" si="0"/>
         <v>-23.614928776430023</v>
       </c>
-      <c r="R16">
+      <c r="R16" s="23">
         <f t="shared" si="0"/>
         <v>-16.964330062819261</v>
       </c>
-      <c r="S16">
+      <c r="S16" s="23">
         <f t="shared" si="0"/>
         <v>-20.512556348769913</v>
       </c>
-      <c r="T16">
+      <c r="T16" s="23">
         <f t="shared" si="0"/>
         <v>-22.524669621589222</v>
       </c>
-      <c r="U16">
+      <c r="U16" s="22">
         <f t="shared" si="0"/>
         <v>-22.445422242164838</v>
       </c>
-      <c r="V16">
+      <c r="V16" s="22">
         <f t="shared" si="0"/>
         <v>-24.683174896031996</v>
       </c>
-      <c r="W16">
+      <c r="W16" s="22">
         <f t="shared" si="0"/>
         <v>-31.305765433684865</v>
       </c>
-      <c r="X16">
+      <c r="X16" s="22">
         <f t="shared" si="0"/>
         <v>-24.076391978101967</v>
       </c>
@@ -12179,70 +12366,70 @@
       <c r="B17" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="20">
         <v>-5.6921999999999997</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="20">
         <v>-5.6460999999999997</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="20">
         <v>-10.119</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="20">
         <v>-13.0959</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="20">
         <v>-14.3096</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="20">
         <v>-16.988900000000001</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="20">
         <v>-20.5703</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="20">
         <v>-22.3443</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="21">
         <v>-21.6006</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="21">
         <v>-26.778199999999998</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="21">
         <v>-29.898900000000001</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="21">
         <v>-17.993400000000001</v>
       </c>
-      <c r="O17">
+      <c r="O17" s="21">
         <v>-21.352</v>
       </c>
-      <c r="P17">
+      <c r="P17" s="21">
         <v>-14.3414</v>
       </c>
-      <c r="Q17">
+      <c r="Q17" s="21">
         <v>-22.144400000000001</v>
       </c>
-      <c r="R17">
+      <c r="R17" s="21">
         <v>-15.975199999999999</v>
       </c>
-      <c r="S17">
+      <c r="S17" s="21">
         <v>-19.305199999999999</v>
       </c>
-      <c r="T17">
+      <c r="T17" s="21">
         <v>-21.282</v>
       </c>
-      <c r="U17">
-        <v>-219932</v>
-      </c>
-      <c r="V17">
+      <c r="U17" s="20">
+        <v>-21.993200000000002</v>
+      </c>
+      <c r="V17" s="20">
         <v>-24.202500000000001</v>
       </c>
-      <c r="W17">
+      <c r="W17" s="20">
         <v>-30.650400000000001</v>
       </c>
-      <c r="X17">
+      <c r="X17" s="20">
         <v>-23.6068</v>
       </c>
     </row>

</xml_diff>